<commit_message>
:cop: getting coverage up to 99.9%
</commit_message>
<xml_diff>
--- a/tests/test-data/ground_truth.xlsx
+++ b/tests/test-data/ground_truth.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rturnbull/MDAP/rdgai/tests/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18E4C32D-7610-EB4E-A375-2333F254457B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F71458E-0FEF-6F46-B831-F56B13BB1426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>App ID</t>
   </si>
@@ -112,6 +112,12 @@
   </si>
   <si>
     <t>category3</t>
+  </si>
+  <si>
+    <t>description1</t>
+  </si>
+  <si>
+    <t>description2</t>
   </si>
 </sst>
 </file>
@@ -130,6 +136,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -457,15 +464,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -485,10 +492,13 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -508,10 +518,13 @@
         <v>12</v>
       </c>
       <c r="G2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -531,10 +544,13 @@
         <v>15</v>
       </c>
       <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -553,17 +569,18 @@
       <c r="F4" t="s">
         <v>15</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" sqref="G2:P5" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" sqref="H2:Q5" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"category1,category2,category3"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -603,11 +620,11 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <f>COUNTIF(Variants!G:P, "category1")</f>
+        <f>COUNTIF(Variants!H:Q, "category1")</f>
         <v>1</v>
       </c>
       <c r="D2">
-        <f>COUNTIF(Variants!G:P, "category1")</f>
+        <f>COUNTIF(Variants!H:Q, "category1")</f>
         <v>1</v>
       </c>
       <c r="E2">
@@ -626,11 +643,11 @@
         <v>16</v>
       </c>
       <c r="C3">
-        <f>COUNTIF(Variants!G:P, "category2")</f>
+        <f>COUNTIF(Variants!H:Q, "category2")</f>
         <v>1</v>
       </c>
       <c r="D3">
-        <f>COUNTIF(Variants!G:P, "category2")</f>
+        <f>COUNTIF(Variants!H:Q, "category2")</f>
         <v>1</v>
       </c>
       <c r="E3">
@@ -649,11 +666,11 @@
         <v>25</v>
       </c>
       <c r="C4">
-        <f>COUNTIF(Variants!G:P, "category3")</f>
+        <f>COUNTIF(Variants!H:Q, "category3")</f>
         <v>1</v>
       </c>
       <c r="D4">
-        <f>COUNTIF(Variants!G:P, "category3")</f>
+        <f>COUNTIF(Variants!H:Q, "category3")</f>
         <v>1</v>
       </c>
       <c r="E4">

</xml_diff>